<commit_message>
I think it is done The date needs to do the "text to column" thing
</commit_message>
<xml_diff>
--- a/Vehicle information_20240816_223858.xlsx
+++ b/Vehicle information_20240816_223858.xlsx
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Arial"/>
@@ -79,7 +81,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -90,6 +92,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>